<commit_message>
Added one click run script so I stop losing it
</commit_message>
<xml_diff>
--- a/Twilight Imperium Data.xlsx
+++ b/Twilight Imperium Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
   <si>
     <t>Game</t>
   </si>
@@ -730,70 +730,158 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="3">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="3">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="3">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="3">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="A49" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="3">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="3">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="3">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="3"/>

</xml_diff>